<commit_message>
Added 5-61, statement of operating expenses. Now doing 5-62...
</commit_message>
<xml_diff>
--- a/Chapter 5/5-61.xlsx
+++ b/Chapter 5/5-61.xlsx
@@ -1,27 +1,117 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\OneDrive\Desktop\Introduction to Financial Accounting\Chapter 5\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58959FE5-24A4-4C56-8714-3701E4F66FAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Statement of Operating Expenses" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+  <si>
+    <t>Name : Clorox Co.</t>
+  </si>
+  <si>
+    <t>Particulars</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>Component</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Dec 31, 2011</t>
+  </si>
+  <si>
+    <t>STATEMENT OF OPERATING EXPENSES (in millions of $)</t>
+  </si>
+  <si>
+    <t>Net Income for 2011</t>
+  </si>
+  <si>
+    <t>Adjustment to reconcile net income</t>
+  </si>
+  <si>
+    <t>to net cash provided by operations:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Income changes not affecting cash:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          Depreciation &amp; amortization</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          Other net non-cash expenses </t>
+  </si>
+  <si>
+    <t xml:space="preserve">          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Changes in assets &amp; liabilities:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          Decrease in Amounts Recievable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          Increase  in Accounts Payable </t>
+  </si>
+  <si>
+    <t xml:space="preserve">          Increase  in Inventories</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          Increase  in Income Taxes Payable</t>
+  </si>
+  <si>
+    <t>Net cash provided by Operations</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -49,8 +139,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,13 +430,147 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="H4:L25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="M23" sqref="M23"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="8" max="8" width="28.33203125" customWidth="1"/>
+    <col min="10" max="10" width="2.21875" customWidth="1"/>
+    <col min="11" max="11" width="15.33203125" customWidth="1"/>
+    <col min="12" max="12" width="11.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="8:12" x14ac:dyDescent="0.3">
+      <c r="J4" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="8:12" x14ac:dyDescent="0.3">
+      <c r="H6" t="s">
+        <v>0</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="8:12" x14ac:dyDescent="0.3">
+      <c r="K7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L7" s="3"/>
+    </row>
+    <row r="8" spans="8:12" x14ac:dyDescent="0.3">
+      <c r="H8" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="I8" s="3"/>
+      <c r="K8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="8:12" x14ac:dyDescent="0.3">
+      <c r="H10" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="L10" s="4">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="12" spans="8:12" x14ac:dyDescent="0.3">
+      <c r="H12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="8:12" x14ac:dyDescent="0.3">
+      <c r="H13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="8:12" x14ac:dyDescent="0.3">
+      <c r="H15" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="8:12" x14ac:dyDescent="0.3">
+      <c r="H16" t="s">
+        <v>11</v>
+      </c>
+      <c r="L16">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="17" spans="8:12" x14ac:dyDescent="0.3">
+      <c r="H17" t="s">
+        <v>12</v>
+      </c>
+      <c r="L17">
+        <v>-21</v>
+      </c>
+    </row>
+    <row r="18" spans="8:12" x14ac:dyDescent="0.3">
+      <c r="H18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="8:12" x14ac:dyDescent="0.3">
+      <c r="H19" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="8:12" x14ac:dyDescent="0.3">
+      <c r="H20" t="s">
+        <v>15</v>
+      </c>
+      <c r="L20">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="8:12" x14ac:dyDescent="0.3">
+      <c r="H21" t="s">
+        <v>17</v>
+      </c>
+      <c r="L21">
+        <v>-65</v>
+      </c>
+    </row>
+    <row r="22" spans="8:12" x14ac:dyDescent="0.3">
+      <c r="H22" t="s">
+        <v>16</v>
+      </c>
+      <c r="L22">
+        <v>-136</v>
+      </c>
+    </row>
+    <row r="23" spans="8:12" x14ac:dyDescent="0.3">
+      <c r="H23" t="s">
+        <v>18</v>
+      </c>
+      <c r="L23">
+        <v>-11</v>
+      </c>
+    </row>
+    <row r="25" spans="8:12" x14ac:dyDescent="0.3">
+      <c r="H25" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="L25" s="4">
+        <f>SUM(L10:L24)</f>
+        <v>126</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="H8:I8"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>